<commit_message>
add combined annual hydrograph plotting
</commit_message>
<xml_diff>
--- a/Scenarios_list.xlsx
+++ b/Scenarios_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noellepatterson/apps/Other/Climate_change_research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08B7883C-F252-B443-823F-5C1FCD6C900A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB24048-3231-C64F-A517-6C7CE0A58420}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1880" yWindow="460" windowWidth="20360" windowHeight="16660" xr2:uid="{C6ACD654-75F0-344B-8E03-DA769AD3D29B}"/>
+    <workbookView xWindow="9580" yWindow="1860" windowWidth="19220" windowHeight="13160" xr2:uid="{C6ACD654-75F0-344B-8E03-DA769AD3D29B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>wet season precip (%)</t>
   </si>
@@ -97,7 +97,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -109,6 +109,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,9 +141,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E470E9EF-5EE2-ED43-900F-F3C996FAD78A}">
   <dimension ref="A2:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="97" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,11 +530,11 @@
       <c r="G7">
         <v>0.70440000000000003</v>
       </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" t="s">
-        <v>11</v>
+      <c r="H7">
+        <v>-0.26355567099999999</v>
+      </c>
+      <c r="I7">
+        <v>-0.138900206</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -548,11 +556,11 @@
       <c r="G8">
         <v>0.85907800000000001</v>
       </c>
-      <c r="H8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" t="s">
-        <v>11</v>
+      <c r="H8">
+        <v>3.7709018888888897E-2</v>
+      </c>
+      <c r="I8">
+        <v>5.2831841111111118E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -571,11 +579,11 @@
       <c r="F9">
         <v>0.26519999999999999</v>
       </c>
-      <c r="H9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" t="s">
-        <v>11</v>
+      <c r="H9">
+        <v>-8.1952915000000001E-2</v>
+      </c>
+      <c r="I9">
+        <v>0.222177229</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -594,11 +602,11 @@
       <c r="F10">
         <v>9.0480000000000005E-2</v>
       </c>
-      <c r="H10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" t="s">
-        <v>11</v>
+      <c r="H10">
+        <v>0.26355567099999999</v>
+      </c>
+      <c r="I10">
+        <v>-0.138900206</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -620,11 +628,11 @@
       <c r="G11">
         <v>0.90642</v>
       </c>
-      <c r="H11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" t="s">
-        <v>11</v>
+      <c r="H11">
+        <v>3.7709018888888897E-2</v>
+      </c>
+      <c r="I11" s="2">
+        <v>5.2831840999999997E-2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -646,11 +654,11 @@
       <c r="G12">
         <v>1.1408999999999998</v>
       </c>
-      <c r="H12" t="s">
-        <v>11</v>
-      </c>
-      <c r="I12" t="s">
-        <v>11</v>
+      <c r="H12">
+        <v>8.1952915000000001E-2</v>
+      </c>
+      <c r="I12">
+        <v>0.222177229</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>